<commit_message>
pairplot and cleaned up some figs
</commit_message>
<xml_diff>
--- a/data/Vader-province_sentiment-correlation.xlsx
+++ b/data/Vader-province_sentiment-correlation.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -54,18 +54,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -486,22 +486,22 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8351128293618785</v>
+        <v>0.3807625718760089</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3882154139868831</v>
+        <v>0.3029493016797381</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6843903710485125</v>
+        <v>0.8249848017418434</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7611841799386381</v>
+        <v>0.5381002104292207</v>
       </c>
       <c r="G2" t="n">
-        <v>0.4264217463555484</v>
+        <v>-0.5925727588665705</v>
       </c>
       <c r="H2" t="n">
-        <v>0.4972657781835089</v>
+        <v>0.8407293522681448</v>
       </c>
     </row>
     <row r="3">
@@ -511,25 +511,25 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8351128293618785</v>
+        <v>0.3807625718760089</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.4873968141252499</v>
+        <v>0.9323058924499702</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7489788003165152</v>
+        <v>0.7075058901348336</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7623414259136896</v>
+        <v>0.6315326640533218</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5301419553498137</v>
+        <v>0.3596764627439427</v>
       </c>
       <c r="H3" t="n">
-        <v>0.5459102691204253</v>
+        <v>0.6056155656471309</v>
       </c>
     </row>
     <row r="4">
@@ -539,25 +539,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.3882154139868831</v>
+        <v>0.3029493016797381</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4873968141252499</v>
+        <v>0.9323058924499702</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4554794462615966</v>
+        <v>0.6569309222873292</v>
       </c>
       <c r="F4" t="n">
-        <v>0.4113521252073592</v>
+        <v>0.6043609692055382</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1649173509847513</v>
+        <v>0.2820080977645044</v>
       </c>
       <c r="H4" t="n">
-        <v>0.436051676731523</v>
+        <v>0.5094350468276497</v>
       </c>
     </row>
     <row r="5">
@@ -567,25 +567,25 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.6843903710485125</v>
+        <v>0.8249848017418434</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7489788003165152</v>
+        <v>0.7075058901348336</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4554794462615966</v>
+        <v>0.6569309222873292</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7068566014693257</v>
+        <v>0.753748537200926</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5473397560293946</v>
+        <v>-0.3177175246249234</v>
       </c>
       <c r="H5" t="n">
-        <v>0.4929171340535298</v>
+        <v>0.9049110834301681</v>
       </c>
     </row>
     <row r="6">
@@ -595,25 +595,25 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.7611841799386381</v>
+        <v>0.5381002104292207</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7623414259136896</v>
+        <v>0.6315326640533218</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4113521252073592</v>
+        <v>0.6043609692055382</v>
       </c>
       <c r="E6" t="n">
-        <v>0.7068566014693257</v>
+        <v>0.753748537200926</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.715033411982409</v>
+        <v>0.1143943837807325</v>
       </c>
       <c r="H6" t="n">
-        <v>0.3452469636641346</v>
+        <v>0.723991459312084</v>
       </c>
     </row>
     <row r="7">
@@ -623,25 +623,25 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.4264217463555484</v>
+        <v>-0.5925727588665705</v>
       </c>
       <c r="C7" t="n">
-        <v>0.5301419553498137</v>
+        <v>0.3596764627439427</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1649173509847513</v>
+        <v>0.2820080977645044</v>
       </c>
       <c r="E7" t="n">
-        <v>0.5473397560293946</v>
+        <v>-0.3177175246249234</v>
       </c>
       <c r="F7" t="n">
-        <v>0.715033411982409</v>
+        <v>0.1143943837807325</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.1087317780465653</v>
+        <v>-0.3014711968983573</v>
       </c>
     </row>
     <row r="8">
@@ -651,28 +651,28 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4972657781835089</v>
+        <v>0.8407293522681448</v>
       </c>
       <c r="C8" t="n">
-        <v>0.5459102691204253</v>
+        <v>0.6056155656471309</v>
       </c>
       <c r="D8" t="n">
-        <v>0.436051676731523</v>
+        <v>0.5094350468276497</v>
       </c>
       <c r="E8" t="n">
-        <v>0.4929171340535298</v>
+        <v>0.9049110834301681</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3452469636641346</v>
+        <v>0.723991459312084</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.1087317780465653</v>
+        <v>-0.3014711968983573</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>